<commit_message>
Update auto calibration 'all' to use meta y factor
</commit_message>
<xml_diff>
--- a/tests/databooks/databook_sir_twopop.xlsx
+++ b/tests/databooks/databook_sir_twopop.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50400C4-12B5-4D09-A826-0DE80603096E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A8EBF7-E1FD-4140-8F52-4A035626D9E1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="3" r:id="rId2"/>
     <sheet name="State Variables" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -445,9 +445,6 @@
     <t>Transmission probability per contact</t>
   </si>
   <si>
-    <t>Quantity Type</t>
-  </si>
-  <si>
     <t>Constant</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>Children</t>
+  </si>
+  <si>
+    <t>Units</t>
   </si>
 </sst>
 </file>
@@ -913,18 +913,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -937,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,10 +953,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1">
         <v>2000</v>
@@ -1022,13 +1022,13 @@
         <v>adults</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1037,24 +1037,24 @@
         <v>children</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E5" s="1">
         <v>2000</v>
@@ -1120,14 +1120,14 @@
         <v>adults</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <f>IF(SUMPRODUCT(--(E6:W6&lt;&gt;""))=0,80,"N.A.")</f>
         <v>80</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1136,25 +1136,25 @@
         <v>children</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <f>IF(SUMPRODUCT(--(E7:W7&lt;&gt;""))=0,80,"N.A.")</f>
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E9" s="1">
         <v>2000</v>
@@ -1220,13 +1220,13 @@
         <v>adults</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1235,24 +1235,24 @@
         <v>children</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E13" s="1">
         <v>2000</v>
@@ -1318,14 +1318,14 @@
         <v>adults</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <f>IF(SUMPRODUCT(--(E14:W14&lt;&gt;""))=0,0.016,"N.A.")</f>
         <v>1.6E-2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1334,25 +1334,25 @@
         <v>children</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <f>IF(SUMPRODUCT(--(E15:W15&lt;&gt;""))=0,0.016,"N.A.")</f>
         <v>1.6E-2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E17" s="1">
         <v>2000</v>
@@ -1418,14 +1418,14 @@
         <v>adults</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <f>IF(SUMPRODUCT(--(E18:W18&lt;&gt;""))=0,0.008,"N.A.")</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -1434,14 +1434,14 @@
         <v>children</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <f>IF(SUMPRODUCT(--(E19:W19&lt;&gt;""))=0,0.008,"N.A.")</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
@@ -1478,13 +1478,13 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1">
         <v>2000</v>
@@ -1550,13 +1550,13 @@
         <v>adults</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>700</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1565,10 +1565,10 @@
         <v>children</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <f>E7*(1-E11)</f>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E5" s="1">
         <v>2000</v>
@@ -1649,13 +1649,13 @@
         <v>adults</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>1000</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -1664,10 +1664,10 @@
         <v>children</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>500</v>
@@ -1675,13 +1675,13 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E9" s="1">
         <v>2000</v>
@@ -1747,13 +1747,13 @@
         <v>adults</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>0.2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <v>0.28571428999999998</v>
@@ -1819,14 +1819,14 @@
         <v>children</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <f>C10*1.5</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>0.4</v>

</xml_diff>